<commit_message>
Analysis pipeline, Manuscript, Suppelements
</commit_message>
<xml_diff>
--- a/paper/tables.xlsx
+++ b/paper/tables.xlsx
@@ -415,7 +415,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +448,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Hospitalization – survey time, days</t>
+          <t>Ward – survey time, days</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -461,7 +461,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Age, accident, years</t>
+          <t>Age, years</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -474,191 +474,167 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Age class</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>young: 20% (n = 61)
+middle: 66% (n = 202)
+elderly: 14% (n = 44)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>female: 45% (n = 137)
 male: 55% (n = 170)</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Residence in the Alps</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>73% (n = 225)</t>
-        </is>
-      </c>
-    </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Residence in the Alps</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>73% (n = 225)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>primary: 3.3% (n = 10)
-apprenticeship: 13% (n = 39)
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>primary/apprenticeship: 16% (n = 49)
 secondary: 38% (n = 115)
 tertiary: 45% (n = 136)</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Employment</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>employed: 68% (n = 210)
-household: 3.3% (n = 10)
-unemployed: 0.33% (n = 1)
+unemployed: 3.6% (n = 11)
 student: 10% (n = 32)
 retired: 18% (n = 54)</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sport profession</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>5.2% (n = 16)</t>
-        </is>
-      </c>
-    </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Trauma-risk profession</t>
+          <t>Sport profession</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7.2% (n = 22)</t>
+          <t>5.2% (n = 16)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Income/year</t>
+          <t>Trauma-risk profession</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>no income: 21% (n = 63)
-&lt; 15000 Euro: 5.5% (n = 17)
-15000 - 30000 Euro: 13% (n = 39)
-30000 - 45000 Euro: 19% (n = 59)
-&gt; 45000 Euro: 42% (n = 129)</t>
+          <t>7.2% (n = 22)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Smoking</t>
+          <t>Income/year</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7.8% (n = 24)</t>
+          <t>no income: 21% (n = 63)
+&lt; 30000 EUR: 18% (n = 56)
+30000 - 45000 EUR: 19% (n = 59)
+≥ 45000 EUR: 42% (n = 129)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Drug consumption</t>
+          <t>Smoking</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2.3% (n = 7)</t>
+          <t>7.8% (n = 24)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Somatic comorbidity</t>
+          <t>Substance abuse (CAGE ≥2)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15% (n = 47)</t>
+          <t>9.4% (n = 29)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mental illness</t>
+          <t>Somatic illness</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5.2% (n = 16)</t>
+          <t>15% (n = 47)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Traumatic event before/DIA-X</t>
+          <t>Mental illness</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>40% (n = 124)</t>
+          <t>5.2% (n = 16)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Self-reported traumatic event type</t>
+          <t>Prior traumatic event/DIA-X</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>none: 88% (n = 271)
-severe accident: 6.2% (n = 19)
-physical assult: 1.6% (n = 5)
-sexual molestation: 0.65% (n = 2)
-rape: 0.33% (n = 1)
-severe disease: 2% (n = 6)
-natural diseaster: 0.65% (n = 2)
-war: 0.33% (n = 1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Self-reported traumatic event past</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>no trauma event: 88% (n = 271)
-0 – 1 years ago: 0.33% (n = 1)
-1 – 5 years ago: 3.9% (n = 12)
-5 – 10 years ago: 1.3% (n = 4)
-10+ years ago: 6.2% (n = 19)</t>
+          <t>40% (n = 124)</t>
         </is>
       </c>
     </row>
@@ -669,7 +645,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -739,11 +715,7 @@
       <c r="B5" t="inlineStr">
         <is>
           <t>self: 77% (n = 237)
-tour partner: 1.3% (n = 4)
-third party: 8.1% (n = 25)
-blow of fate: 3.9% (n = 12)
-natural diseaster: 0.65% (n = 2)
-other reason: 8.8% (n = 27)
+non-self: 23% (n = 70)
 n = 307</t>
         </is>
       </c>
@@ -756,10 +728,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>only self: 93% (n = 195)
-self and partner: 5.2% (n = 11)
-3+ persons: 1.9% (n = 4)
-n = 210</t>
+          <t>only self: 64% (n = 195)
+self and partner: 3.6% (n = 11)
+3+ persons: 1.3% (n = 4)
+no information: 32% (n = 97)
+n = 307</t>
         </is>
       </c>
     </row>
@@ -772,9 +745,8 @@
       <c r="B7" t="inlineStr">
         <is>
           <t>self: 50% (n = 155)
-tour partner: 13% (n = 39)
+partner/third party: 21% (n = 63)
 rescue team: 29% (n = 89)
-third party: 7.8% (n = 24)
 n = 307</t>
         </is>
       </c>
@@ -782,27 +754,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Injury severity class, AIS score</t>
+          <t>Injury severity, AIS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1: 37% (n = 104)
-2: 33% (n = 93)
-3+: 29% (n = 82)
-n = 279</t>
+          <t>1: 37% (n = 108)
+2: 35% (n = 103)
+3+: 28% (n = 83)
+n = 294</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Psychological support</t>
+          <t>Hospitalized</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5.2% (n = 16)
+          <t>26% (n = 80)
 n = 307</t>
         </is>
       </c>
@@ -810,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Somatic accident aftermath</t>
+          <t>Surgery</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>37% (n = 115)
+          <t>14% (n = 43)
 n = 307</t>
         </is>
       </c>
@@ -823,12 +795,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Returned to same sport</t>
+          <t>Psychological support</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>85% (n = 262)
+          <t>9.1% (n = 28)
 n = 307</t>
         </is>
       </c>
@@ -836,14 +808,68 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Behavior post accident</t>
+          <t>Psychological support need</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
+        <is>
+          <t>7.5% (n = 23)
+n = 307</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Somatic accident aftermath</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>37% (n = 115)
+n = 307</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Returned to same sport</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>85% (n = 262)
+n = 307</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Caution post accident</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>no change: 35% (n = 106)
 more cautious: 65% (n = 199)
 less cautious: 0.65% (n = 2)
+n = 307</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Flashback frequency</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>none: 60% (n = 185)
+&gt; 1/month: 18% (n = 54)
+&gt; 1/year: 22% (n = 68)
 n = 307</t>
         </is>
       </c>
@@ -855,7 +881,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -888,137 +914,124 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PSS4 score</t>
+          <t>GAD-7 score</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4 [IQR: 3 - 6]
-range: 0 - 14</t>
+          <t>1 [IQR: 0 - 3]
+range: 0 - 15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GAD-7 score</t>
+          <t>Anxiety symptoms (GAD-7 ≥10)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1 [IQR: 0 - 3]
-range: 0 - 15</t>
+          <t>2.3% (n = 7)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anxiety+ (GAD-7 ≥10)</t>
+          <t>PHQ-9 score</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2.3% (n = 7)</t>
+          <t>2 [IQR: 1 - 5]
+range: 0 - 16</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PHQ-9 score</t>
+          <t>Depression symptoms (PHQ-9 ≥11)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2 [IQR: 1 - 5]
-range: 0 - 16</t>
+          <t>5.5% (n = 17)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Depression+ (PHQ-9 ≥11)</t>
+          <t>PHQ-15 score</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5.5% (n = 17)</t>
+          <t>2 [IQR: 1 - 4]
+range: 0 - 23</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PHQ-15 score</t>
+          <t>Somatization symptoms (PHQ-15 ≥11)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2 [IQR: 1 - 4]
-range: 0 - 23</t>
+          <t>4.9% (n = 15)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Somatization+ (PHQ-15 ≥11)</t>
+          <t>EUROHIS-QOL 8 score</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4.9% (n = 15)</t>
+          <t>1.6 [IQR: 1.4 - 2]
+range: 1 - 4</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EUROHIS-QOL 8 score</t>
+          <t>SOC-9L score</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.6 [IQR: 1.4 - 2]
-range: 1 - 4</t>
+          <t>19 [IQR: 16 - 25]
+range: 10 - 49</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SOC-9L score</t>
+          <t>RS13 score</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>19 [IQR: 16 - 25]
-range: 10 - 49</t>
+          <t>78 [IQR: 70 - 85]
+range: 15 - 91</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RS13 score</t>
+          <t>RS13 coping class</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
-        <is>
-          <t>78 [IQR: 70 - 85]
-range: 15 - 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RS13 coping class</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
         <is>
           <t>low: 18% (n = 56)
 moderate: 14% (n = 42)
@@ -1026,69 +1039,41 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PTGI score</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>32 [IQR: 16 - 48]
+range: 0 - 100</t>
+        </is>
+      </c>
+    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Abuse+ (CAGE ≥2)</t>
+          <t>PCL-5 DSM-5 score</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>9.4% (n = 29)</t>
+          <t>3 [IQR: 1 - 7]
+range: 0 - 44</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Flashback frequency</t>
+          <t>PTSD+ (at least one domain)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>no flashbacks: 60% (n = 185)
-&gt; 1 – 2 per week: 2.6% (n = 8)
-several per month: 5.2% (n = 16)
-1 – 2 per month: 9.8% (n = 30)
-1 – 2 per year: 22% (n = 68)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>PCL-5 DSM-5 score</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3 [IQR: 1 - 7]
-range: 0 - 44</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>PTSD+ (at least one cluster)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
           <t>19% (n = 58)</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>PTGI score</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>32 [IQR: 16 - 48]
-range: 0 - 100</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes in figures, tables and paper text
Changes in the table layout, shortening of the text, focus on early predictors of mental problems post accident
</commit_message>
<xml_diff>
--- a/paper/tables.xlsx
+++ b/paper/tables.xlsx
@@ -474,14 +474,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Age class</t>
+          <t>Age class, years</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>young: 20% (n = 61)
-middle: 66% (n = 202)
-elderly: 14% (n = 44)</t>
+          <t>16-30: 20% (n = 61)
+31-65: 66% (n = 202)
+&gt;65: 14% (n = 44)</t>
         </is>
       </c>
     </row>
@@ -605,12 +605,20 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pre-existing somatic illness</t>
+          <t>Pre-existing somatic illness type</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15% (n = 47)</t>
+          <t>none: 85% (n = 260)
+CVD: 2.9% (n = 9)
+neurological: 1.3% (n = 4)
+metabolic: 1.3% (n = 4)
+pulmonary: 0.65% (n = 2)
+cancer: 0.65% (n = 2)
+rheumatoid: 0.33% (n = 1)
+skin: 0.33% (n = 1)
+other: 7.8% (n = 24)</t>
         </is>
       </c>
     </row>
@@ -686,7 +694,7 @@
         <is>
           <t>ski/snowboard: 64% (n = 197)
 sledding: 3.9% (n = 12)
-mountain: 14% (n = 42)
+climbing/hiking/mountaineering: 14% (n = 42)
 biking: 16% (n = 48)
 other: 2.6% (n = 8)
 n = 307</t>
@@ -994,8 +1002,8 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.6 [IQR: 1.4 - 2]
-range: 1 - 4</t>
+          <t>4.4 [IQR: 4 - 4.6]
+range: 2 - 5</t>
         </is>
       </c>
     </row>

</xml_diff>